<commit_message>
1st and Last occurance added and 450 updated
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="477">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1455,6 +1455,9 @@
   </si>
   <si>
     <t>Iter,Recursive done</t>
+  </si>
+  <si>
+    <t>Iterative binary search modification done</t>
   </si>
 </sst>
 </file>
@@ -1812,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C99" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2855,7 +2858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>54</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>54</v>
       </c>
@@ -2877,24 +2880,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
       <c r="B100" s="8"/>
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
+    <row r="101" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C101" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C101" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>98</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>98</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>98</v>
       </c>
@@ -2927,7 +2933,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>98</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>98</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>98</v>
       </c>
@@ -2960,7 +2966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>98</v>
       </c>
@@ -2971,7 +2977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>98</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>98</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>98</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
largestSum,Find first last,interlivingstring,string rotate, 450 updated
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="481">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1458,6 +1458,18 @@
   </si>
   <si>
     <t>Iterative binary search modification done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To be read </t>
+  </si>
+  <si>
+    <t>String Methods</t>
+  </si>
+  <si>
+    <t>One Done, Another one is there in Dynamic Programming</t>
+  </si>
+  <si>
+    <t>Also Known As KADANE's algo</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1543,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1541,6 +1553,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1557,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1598,6 +1616,15 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1815,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C99" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1953,15 +1980,18 @@
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
+      <c r="C13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2440,37 +2470,43 @@
         <v>470</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
+    <row r="59" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
+      <c r="C59" s="20" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+      <c r="C60" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>5</v>
+      <c r="C61" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
stack class created and 450 updated
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="484">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1476,6 +1476,9 @@
   </si>
   <si>
     <t>Starting return and ending return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arraylist Based </t>
   </si>
 </sst>
 </file>
@@ -1861,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="D299" sqref="D299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4944,7 +4947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A289" s="6" t="s">
         <v>266</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A290" s="6" t="s">
         <v>266</v>
       </c>
@@ -4966,7 +4969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A291" s="6" t="s">
         <v>266</v>
       </c>
@@ -4977,7 +4980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A292" s="6" t="s">
         <v>266</v>
       </c>
@@ -4988,7 +4991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A293" s="6" t="s">
         <v>266</v>
       </c>
@@ -4999,26 +5002,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B294" s="8"/>
       <c r="C294" s="5"/>
     </row>
-    <row r="295" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B295" s="8"/>
       <c r="C295" s="5"/>
     </row>
-    <row r="296" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A296" s="6" t="s">
+    <row r="296" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A296" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B296" s="7" t="s">
+      <c r="B296" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="C296" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C296" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D296" s="13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A297" s="6" t="s">
         <v>286</v>
       </c>
@@ -5029,7 +5035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A298" s="6" t="s">
         <v>286</v>
       </c>
@@ -5040,7 +5046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A299" s="6" t="s">
         <v>286</v>
       </c>
@@ -5051,7 +5057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A300" s="6" t="s">
         <v>286</v>
       </c>
@@ -5062,7 +5068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A301" s="6" t="s">
         <v>286</v>
       </c>
@@ -5073,7 +5079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A302" s="6" t="s">
         <v>286</v>
       </c>
@@ -5084,7 +5090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A303" s="6" t="s">
         <v>286</v>
       </c>
@@ -5095,7 +5101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A304" s="6" t="s">
         <v>286</v>
       </c>

</xml_diff>

<commit_message>
stack and queue added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="486">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1482,6 +1482,9 @@
   </si>
   <si>
     <t>Efficient Circular Queue based</t>
+  </si>
+  <si>
+    <t>Efficient array based implementation</t>
   </si>
 </sst>
 </file>
@@ -1593,7 +1596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1650,7 +1653,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
-      <selection activeCell="D303" sqref="D303"/>
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="D298" sqref="D298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5014,43 +5016,46 @@
       <c r="B295" s="8"/>
       <c r="C295" s="5"/>
     </row>
-    <row r="296" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A296" s="18" t="s">
+    <row r="296" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B296" s="26" t="s">
+      <c r="B296" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="C296" s="20" t="s">
+      <c r="C296" s="15" t="s">
         <v>465</v>
       </c>
-      <c r="D296" s="21" t="s">
+      <c r="D296" s="13" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="297" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="18" t="s">
+    <row r="297" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B297" s="26" t="s">
+      <c r="B297" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="C297" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D297" s="21" t="s">
+      <c r="C297" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D297" s="13" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="6" t="s">
+    <row r="298" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A298" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B298" s="7" t="s">
+      <c r="B298" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="C298" s="5" t="s">
-        <v>5</v>
+      <c r="C298" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D298" s="13" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
BinarySearch in matrix added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1596,7 +1596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1653,10 +1653,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1874,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2347,26 +2343,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="26" t="s">
+    <row r="44" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="C44" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>5</v>
+      <c r="C45" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Coin Change Minimum Problem Added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D417" sqref="D417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6223,15 +6223,15 @@
       <c r="B409" s="8"/>
       <c r="C409" s="5"/>
     </row>
-    <row r="410" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A410" s="6" t="s">
+    <row r="410" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A410" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="B410" s="7" t="s">
+      <c r="B410" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="C410" s="5" t="s">
-        <v>5</v>
+      <c r="C410" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Minimum Jump Problem added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="488">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1485,6 +1485,12 @@
   </si>
   <si>
     <t>Efficient array based implementation</t>
+  </si>
+  <si>
+    <t>Ambiguity</t>
+  </si>
+  <si>
+    <t>We can Assume that it will always reach at the end of array</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1653,6 +1659,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1871,7 +1885,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D417" sqref="D417"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2022,26 +2036,32 @@
         <v>480</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:4" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="C14" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
+      <c r="C15" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6234,14 +6254,14 @@
         <v>465</v>
       </c>
     </row>
-    <row r="411" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A411" s="6" t="s">
+    <row r="411" spans="1:3" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A411" s="26" t="s">
         <v>394</v>
       </c>
-      <c r="B411" s="7" t="s">
+      <c r="B411" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="C411" s="5" t="s">
+      <c r="C411" s="28" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rat in Maze added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="489">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1491,6 +1491,9 @@
   </si>
   <si>
     <t>We can Assume that it will always reach at the end of array</t>
+  </si>
+  <si>
+    <t>4 functions needed printsol,issafe,solvemaze,solvemazeutil</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2585,14 +2588,14 @@
         <v>482</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:4" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4811,26 +4814,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B273" s="8"/>
       <c r="C273" s="5"/>
     </row>
-    <row r="274" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B274" s="8"/>
       <c r="C274" s="5"/>
     </row>
-    <row r="275" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="6" t="s">
+    <row r="275" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A275" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="B275" s="7" t="s">
+      <c r="B275" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="C275" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C275" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D275" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="6" t="s">
         <v>266</v>
       </c>
@@ -4841,7 +4847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="6" t="s">
         <v>266</v>
       </c>
@@ -4852,7 +4858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="6" t="s">
         <v>266</v>
       </c>
@@ -4863,7 +4869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="6" t="s">
         <v>266</v>
       </c>
@@ -4874,7 +4880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="6" t="s">
         <v>266</v>
       </c>
@@ -4885,7 +4891,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="6" t="s">
         <v>266</v>
       </c>
@@ -4896,7 +4902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="6" t="s">
         <v>266</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="6" t="s">
         <v>266</v>
       </c>
@@ -4918,7 +4924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="6" t="s">
         <v>266</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="6" t="s">
         <v>266</v>
       </c>
@@ -4940,7 +4946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="6" t="s">
         <v>266</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="6" t="s">
         <v>266</v>
       </c>
@@ -4962,7 +4968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="6" t="s">
         <v>266</v>
       </c>

</xml_diff>

<commit_message>
Diameter,inpostpre order, mirror added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="492">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1500,6 +1500,9 @@
   </si>
   <si>
     <t>Maxdepth problem done</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1893,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3829,59 +3832,62 @@
         <v>490</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="6" t="s">
+    <row r="180" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B180" s="7" t="s">
+      <c r="B180" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C180" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="6" t="s">
+      <c r="C180" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D180" s="13" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B181" s="7" t="s">
+      <c r="B181" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C181" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="6" t="s">
+      <c r="C181" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B182" s="7" t="s">
+      <c r="B182" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C182" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="6" t="s">
+      <c r="C182" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B183" s="7" t="s">
+      <c r="B183" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="C183" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="6" t="s">
+      <c r="C183" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B184" s="7" t="s">
+      <c r="B184" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C184" s="5" t="s">
-        <v>5</v>
+      <c r="C184" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Top,bottom,left,right views added and node updated
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1896,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C186" sqref="C186:C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3890,48 +3890,48 @@
         <v>465</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="6" t="s">
+    <row r="185" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B185" s="7" t="s">
+      <c r="B185" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C185" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="6" t="s">
+      <c r="C185" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B186" s="7" t="s">
+      <c r="B186" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C186" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="6" t="s">
+      <c r="C186" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B187" s="7" t="s">
+      <c r="B187" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C187" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="6" t="s">
+      <c r="C187" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B188" s="7" t="s">
+      <c r="B188" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C188" s="5" t="s">
-        <v>5</v>
+      <c r="C188" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
zigzag traversal and balanced binary tree added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1614,7 +1614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1679,6 +1679,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1896,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186:C188"/>
+    <sheetView tabSelected="1" topLeftCell="C185" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C190" sqref="C190:C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3934,36 +3935,36 @@
         <v>465</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="6" t="s">
+    <row r="189" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B189" s="7" t="s">
+      <c r="B189" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C189" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="6" t="s">
+      <c r="C189" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B190" s="7" t="s">
+      <c r="B190" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C190" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="6" t="s">
+      <c r="C190" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B191" s="7" t="s">
+      <c r="B191" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="C191" s="5" t="s">
+      <c r="C191" s="20" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Public Methods made and Search and Insertion in BST added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C185" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190:C191"/>
+    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D216" sqref="D216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4198,15 +4198,15 @@
       <c r="B213" s="8"/>
       <c r="C213" s="5"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="6" t="s">
+    <row r="214" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B214" s="7" t="s">
+      <c r="B214" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="C214" s="5" t="s">
-        <v>5</v>
+      <c r="C214" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Max Min in BST, delete node added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D216" sqref="D216"/>
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4209,36 +4209,36 @@
         <v>465</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="6" t="s">
+    <row r="215" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A215" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B215" s="7" t="s">
+      <c r="B215" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C215" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="6" t="s">
+      <c r="C215" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B216" s="7" t="s">
+      <c r="B216" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C216" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="6" t="s">
+      <c r="C216" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="B217" s="7" t="s">
+      <c r="B217" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="C217" s="5" t="s">
+      <c r="C217" s="20" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Predecessor and Succesor and Valid BST or Not added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1576,7 +1576,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1601,12 +1601,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1620,7 +1614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1686,9 +1680,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1906,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A218" sqref="A218:XFD218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4240,25 +4231,25 @@
         <v>465</v>
       </c>
     </row>
-    <row r="217" spans="1:3" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="31" t="s">
+    <row r="217" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A217" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B217" s="30" t="s">
+      <c r="B217" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C217" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="6" t="s">
+      <c r="C217" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A218" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B218" s="7" t="s">
+      <c r="B218" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="C218" s="5" t="s">
+      <c r="C218" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BST from pre order added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1917,8 +1917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4295,18 +4295,18 @@
         <v>215</v>
       </c>
       <c r="C220" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="6" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B221" s="7" t="s">
+      <c r="B221" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C221" s="5" t="s">
-        <v>5</v>
+      <c r="C221" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
linked list and merge two BST added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="495">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1509,6 +1509,9 @@
   </si>
   <si>
     <t>No company tag</t>
+  </si>
+  <si>
+    <t>Not req for now</t>
   </si>
 </sst>
 </file>
@@ -1923,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B143" sqref="B143"/>
+    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4318,36 +4321,39 @@
         <v>465</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A222" s="6" t="s">
+    <row r="222" spans="1:4" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A222" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="B222" s="7" t="s">
+      <c r="B222" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="C222" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A223" s="6" t="s">
+      <c r="C222" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D222" s="34" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A223" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B223" s="7" t="s">
+      <c r="B223" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="C223" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A224" s="6" t="s">
+      <c r="C223" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A224" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="B224" s="7" t="s">
+      <c r="B224" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C224" s="5" t="s">
+      <c r="C224" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8049,6 +8055,6 @@
     <hyperlink ref="B481" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Boundary traversal and diagonal traversal added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="498">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1518,6 +1518,9 @@
   </si>
   <si>
     <t>Related to Morris Traversal</t>
+  </si>
+  <si>
+    <t>Inclusive high and low</t>
   </si>
 </sst>
 </file>
@@ -1635,7 +1638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1700,7 +1703,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1932,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B232" sqref="B232"/>
+    <sheetView tabSelected="1" topLeftCell="C180" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191:C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2434,7 +2436,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="35" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="27" t="s">
@@ -3443,7 +3445,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="36" t="s">
+      <c r="A140" s="35" t="s">
         <v>135</v>
       </c>
       <c r="B140" s="27" t="s">
@@ -3995,26 +3997,26 @@
         <v>465</v>
       </c>
     </row>
-    <row r="191" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="18" t="s">
+    <row r="191" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B191" s="30" t="s">
+      <c r="B191" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C191" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="6" t="s">
+      <c r="C191" s="15" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B192" s="7" t="s">
+      <c r="B192" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C192" s="5" t="s">
-        <v>5</v>
+      <c r="C192" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4291,17 +4293,17 @@
         <v>465</v>
       </c>
     </row>
-    <row r="219" spans="1:4" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="31" t="s">
+    <row r="219" spans="1:4" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A219" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B219" s="32" t="s">
+      <c r="B219" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C219" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D219" s="34" t="s">
+      <c r="C219" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D219" s="33" t="s">
         <v>492</v>
       </c>
     </row>
@@ -4309,7 +4311,7 @@
       <c r="A220" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B220" s="35" t="s">
+      <c r="B220" s="34" t="s">
         <v>215</v>
       </c>
       <c r="C220" s="15" t="s">
@@ -4327,17 +4329,17 @@
         <v>465</v>
       </c>
     </row>
-    <row r="222" spans="1:4" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="31" t="s">
+    <row r="222" spans="1:4" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A222" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B222" s="32" t="s">
+      <c r="B222" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="C222" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D222" s="34" t="s">
+      <c r="C222" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D222" s="33" t="s">
         <v>494</v>
       </c>
     </row>
@@ -4385,54 +4387,60 @@
         <v>465</v>
       </c>
     </row>
-    <row r="227" spans="1:4" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="31" t="s">
+    <row r="227" spans="1:4" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B227" s="32" t="s">
+      <c r="B227" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="C227" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D227" s="34" t="s">
+      <c r="C227" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D227" s="33" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="228" spans="1:4" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="18" t="s">
+    <row r="228" spans="1:4" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B228" s="30" t="s">
+      <c r="B228" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="C228" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D228" s="21" t="s">
+      <c r="C228" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D228" s="33" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="6" t="s">
+    <row r="229" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B229" s="7" t="s">
+      <c r="B229" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C229" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="6" t="s">
+      <c r="C229" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D229" s="13" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="B230" s="7" t="s">
+      <c r="B230" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="C230" s="5" t="s">
-        <v>5</v>
+      <c r="C230" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D230" s="33" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Search in sorted and rotated array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1934,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C180" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191:C192"/>
+    <sheetView tabSelected="1" topLeftCell="C99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102:C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3054,15 +3054,15 @@
         <v>465</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
+    <row r="103" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C103" s="5" t="s">
-        <v>5</v>
+      <c r="C103" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
duplicate in N+1 array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1638,7 +1638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1717,6 +1717,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1934,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102:C103"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2114,25 +2115,25 @@
         <v>487</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="C16" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3065,25 +3066,25 @@
         <v>465</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="6" t="s">
+    <row r="104" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B104" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="6" t="s">
+      <c r="C104" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B105" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C105" s="5" t="s">
+      <c r="C105" s="15" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Longest rec substr with and without duplicate added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="501">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1521,6 +1521,15 @@
   </si>
   <si>
     <t>Inclusive high and low</t>
+  </si>
+  <si>
+    <t>Hard, need to cross check again</t>
+  </si>
+  <si>
+    <t>Longest string with repeated characters</t>
+  </si>
+  <si>
+    <t>Without Duplicate characters</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1717,7 +1726,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1935,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A403" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D424" sqref="D424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2126,18 +2134,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:4" s="33" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
@@ -2148,7 +2159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>6</v>
       </c>
@@ -2159,7 +2170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
@@ -2170,7 +2181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -2181,7 +2192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
@@ -2192,7 +2203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>6</v>
       </c>
@@ -2203,7 +2214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>6</v>
       </c>
@@ -2214,7 +2225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>6</v>
       </c>
@@ -2225,7 +2236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>6</v>
       </c>
@@ -2236,7 +2247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>6</v>
       </c>
@@ -2247,7 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>6</v>
       </c>
@@ -2258,7 +2269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
@@ -2269,7 +2280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>6</v>
       </c>
@@ -2280,7 +2291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>6</v>
       </c>
@@ -2291,7 +2302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>6</v>
       </c>
@@ -2639,15 +2650,18 @@
         <v>482</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="29" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="26" t="s">
+    <row r="64" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="27" t="s">
+      <c r="B64" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="28" t="s">
-        <v>5</v>
+      <c r="C64" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -6404,7 +6418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="417" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A417" s="6" t="s">
         <v>394</v>
       </c>
@@ -6415,7 +6429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A418" s="6" t="s">
         <v>394</v>
       </c>
@@ -6426,7 +6440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="419" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A419" s="6" t="s">
         <v>394</v>
       </c>
@@ -6437,7 +6451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="420" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A420" s="6" t="s">
         <v>394</v>
       </c>
@@ -6448,7 +6462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="421" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A421" s="6" t="s">
         <v>394</v>
       </c>
@@ -6459,7 +6473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="422" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A422" s="6" t="s">
         <v>394</v>
       </c>
@@ -6470,7 +6484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="423" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A423" s="6" t="s">
         <v>394</v>
       </c>
@@ -6481,18 +6495,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="424" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A424" s="6" t="s">
+    <row r="424" spans="1:4" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A424" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="B424" s="7" t="s">
+      <c r="B424" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="C424" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="425" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C424" s="15" t="s">
+        <v>465</v>
+      </c>
+      <c r="D424" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A425" s="6" t="s">
         <v>394</v>
       </c>
@@ -6503,7 +6520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="426" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A426" s="6" t="s">
         <v>394</v>
       </c>
@@ -6514,7 +6531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="427" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A427" s="6" t="s">
         <v>394</v>
       </c>
@@ -6525,7 +6542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="428" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A428" s="6" t="s">
         <v>394</v>
       </c>
@@ -6536,7 +6553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="429" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A429" s="6" t="s">
         <v>394</v>
       </c>
@@ -6547,7 +6564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="430" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A430" s="6" t="s">
         <v>394</v>
       </c>
@@ -6558,7 +6575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="431" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="6" t="s">
         <v>394</v>
       </c>
@@ -6569,7 +6586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="432" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A432" s="6" t="s">
         <v>394</v>
       </c>

</xml_diff>